<commit_message>
Archivo para el trabajo
</commit_message>
<xml_diff>
--- a/_programacion-R/EjemploBaseDeDatos.xlsx
+++ b/_programacion-R/EjemploBaseDeDatos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Puntos" sheetId="1" state="visible" r:id="rId2"/>
@@ -72,6 +72,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -155,14 +156,14 @@
   </sheetPr>
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="250" zoomScaleNormal="250" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.3622448979592"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.1428571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -225,15 +226,15 @@
   </sheetPr>
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="250" zoomScaleNormal="250" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.6683673469388"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -252,7 +253,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>800234</v>
@@ -593,7 +594,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
@@ -608,15 +609,15 @@
   </sheetPr>
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="250" zoomScaleNormal="250" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.6377551020408"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -930,7 +931,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>

</xml_diff>